<commit_message>
feat(core-lib): 新增 Guard 方法。
</commit_message>
<xml_diff>
--- a/assets/内置资源文件设计.xlsx
+++ b/assets/内置资源文件设计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
   <si>
     <t>Project</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>此方法可能缺少了必需的参数值：{0}。</t>
+  </si>
+  <si>
+    <t>ArgumentNullException_with_method_and_parameter_name</t>
+  </si>
+  <si>
+    <t>The method "{0}" may be missing the required parameter value: {1}.</t>
+  </si>
+  <si>
+    <t>方法 「{0}」 可能缺少了必需的參數值：{1}。</t>
+  </si>
+  <si>
+    <t>方法 “{0}” 可能缺少了必需的参数值：{1}。</t>
   </si>
 </sst>
 </file>
@@ -1268,17 +1280,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1" outlineLevelRow="4" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1" outlineLevelRow="5" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="24.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" style="1" customWidth="1"/>
@@ -1407,6 +1419,29 @@
         <v>25</v>
       </c>
     </row>
+    <row r="6" customHeight="1" spans="1:8">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(core-lib): 为 EmitData 类增加了 AddOptional 和 TryGetOptional 方法。
</commit_message>
<xml_diff>
--- a/assets/内置资源文件设计.xlsx
+++ b/assets/内置资源文件设计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="42">
   <si>
     <t>Project</t>
   </si>
@@ -117,6 +117,42 @@
   </si>
   <si>
     <t>方法 “{0}” 可能缺少了必需的参数值：{1}。</t>
+  </si>
+  <si>
+    <t>ArgumentException_default_message</t>
+  </si>
+  <si>
+    <t>Invalid method parameter value.</t>
+  </si>
+  <si>
+    <t>無效的方法參數值。</t>
+  </si>
+  <si>
+    <t>无效的方法参数值。</t>
+  </si>
+  <si>
+    <t>ArgumentException_with_parameter_name</t>
+  </si>
+  <si>
+    <t>Invalid method parameter value. The parameter name is {0}.</t>
+  </si>
+  <si>
+    <t>無效的方法參數值。 參數名稱為：「{0}」。</t>
+  </si>
+  <si>
+    <t>无效的方法参数值。参数名称为：“{0}”。</t>
+  </si>
+  <si>
+    <t>ArgumentException_with_method_and_parameter_name</t>
+  </si>
+  <si>
+    <t>Invalid method ({0}) parameter value. The parameter name is {1}.</t>
+  </si>
+  <si>
+    <t>無效的方法 （{0}） 參數值。 參數名稱為：「{1}」。</t>
+  </si>
+  <si>
+    <t>无效的方法 （{0}） 参数值。参数名称为：“{1}”。</t>
   </si>
 </sst>
 </file>
@@ -1280,24 +1316,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1" outlineLevelRow="5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="24.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.25" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="50.375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="33.75" style="1" customWidth="1"/>
+    <col min="1" max="8" width="32.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1440,6 +1471,75 @@
       </c>
       <c r="H6" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:8">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:8">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:8">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(common): 新增日期时间 System.DateTime 扩展方法。
</commit_message>
<xml_diff>
--- a/assets/内置资源文件设计.xlsx
+++ b/assets/内置资源文件设计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>Project</t>
   </si>
@@ -177,6 +177,84 @@
   </si>
   <si>
     <t>无效的网络通信端口号 “{0}”。</t>
+  </si>
+  <si>
+    <t>DateTime_GetDescription_just_now</t>
+  </si>
+  <si>
+    <t>1 分钟以内</t>
+  </si>
+  <si>
+    <t>Just now</t>
+  </si>
+  <si>
+    <t>就在剛剛</t>
+  </si>
+  <si>
+    <t>就在刚刚</t>
+  </si>
+  <si>
+    <t>DateTime_GetDescription_minutes</t>
+  </si>
+  <si>
+    <t>60 分钟以内</t>
+  </si>
+  <si>
+    <t>{0} minutes ago</t>
+  </si>
+  <si>
+    <t>{0} 分鐘前</t>
+  </si>
+  <si>
+    <t>{0} 分钟前</t>
+  </si>
+  <si>
+    <t>DateTime_GetDescription_hours</t>
+  </si>
+  <si>
+    <t>24 小时以内</t>
+  </si>
+  <si>
+    <t>{0} hours ago</t>
+  </si>
+  <si>
+    <t>{0} 小時前</t>
+  </si>
+  <si>
+    <t>{0} 小时前</t>
+  </si>
+  <si>
+    <t>DateTime_GetDescription_days</t>
+  </si>
+  <si>
+    <t>180 天以内</t>
+  </si>
+  <si>
+    <t>{0} days ago</t>
+  </si>
+  <si>
+    <t>{0} 天前</t>
+  </si>
+  <si>
+    <t>DateTime_GetDescription_same_year</t>
+  </si>
+  <si>
+    <t>180 天以上且在同一年</t>
+  </si>
+  <si>
+    <t>dd/MM</t>
+  </si>
+  <si>
+    <t>MM月dd日</t>
+  </si>
+  <si>
+    <t>DateTime_GetDescription_default</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>yyyy年MM月dd日</t>
   </si>
 </sst>
 </file>
@@ -1340,14 +1418,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1" outlineLevelCol="7"/>
@@ -1612,6 +1690,159 @@
         <v>49</v>
       </c>
     </row>
+    <row r="12" customHeight="1" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:8">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:8">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:8">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(Common): 新增 Exception 扩展方法。
</commit_message>
<xml_diff>
--- a/assets/内置资源文件设计.xlsx
+++ b/assets/内置资源文件设计.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="108">
   <si>
     <t>Project</t>
   </si>
@@ -327,6 +327,30 @@
   </si>
   <si>
     <t>无效的宏参数名称。您可能提供了字母、数字、英文减号和英文下划线之外的特殊字符。</t>
+  </si>
+  <si>
+    <t>Exception_get_summary_with_reason</t>
+  </si>
+  <si>
+    <t>When "{0}", an exception of type "{1}" is thrown: {2}</t>
+  </si>
+  <si>
+    <t>當 「{0}」 時，引發了一個 「{1}」 類型的異常：{2}</t>
+  </si>
+  <si>
+    <t>当 “{0}” 时，引发了一个 “{1}” 类型的异常：{2}</t>
+  </si>
+  <si>
+    <t>Exception_get_summary_without_reason</t>
+  </si>
+  <si>
+    <t>When method "{0}" is called, an exception of type "{1}" is thrown: {2}</t>
+  </si>
+  <si>
+    <t>當調用方法 「{0}」 時，引發了一個 「{1}」 類型的異常：{2}</t>
+  </si>
+  <si>
+    <t>当调用方法 “{0}” 时，引发了一个 “{1}” 类型的异常：{2}</t>
   </si>
 </sst>
 </file>
@@ -1490,19 +1514,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F8" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="8" width="32.625" style="1" customWidth="1"/>
+    <col min="1" max="2" width="32.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="61.875" style="1" customWidth="1"/>
+    <col min="4" max="8" width="32.625" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2053,6 +2079,52 @@
         <v>99</v>
       </c>
     </row>
+    <row r="24" customHeight="1" spans="1:8">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:8">
+      <c r="A25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>